<commit_message>
Added IRFs and ability to toggle with slide bars. Also added ability to change shock persistence (rho)
</commit_message>
<xml_diff>
--- a/server/econ_model/data/output_data/simulation_full_irfs_weblab.xlsx
+++ b/server/econ_model/data/output_data/simulation_full_irfs_weblab.xlsx
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Q4 2018$</t>
+          <t>Q4 2018</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -482,7 +482,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Q1 2019$</t>
+          <t>Q1 2019</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -501,7 +501,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Q2 2019$</t>
+          <t>Q2 2019</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -520,7 +520,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Q3 2019$</t>
+          <t>Q3 2019</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -539,533 +539,533 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Q4 2019$</t>
+          <t>Q4 2019</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>7.67906559498353</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.5611116717935283</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.2247201262549182</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Q1 2020$</t>
+          <t>Q1 2020</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.126180620310202</v>
+        <v>0.1738722793249711</v>
       </c>
       <c r="C7" t="n">
-        <v>0.784399373242246</v>
+        <v>4.202493577422769</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0573163021242165</v>
+        <v>1.489088372285891</v>
       </c>
       <c r="E7" t="n">
-        <v>0.02295465822097256</v>
+        <v>0.3912824475614967</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Q2 2020$</t>
+          <t>Q2 2020</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.463441331250817</v>
+        <v>0.5150643219552331</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9466820060198631</v>
+        <v>2.38438084022046</v>
       </c>
       <c r="D8" t="n">
-        <v>0.189914111213229</v>
+        <v>1.085193212321585</v>
       </c>
       <c r="E8" t="n">
-        <v>0.05511001274358935</v>
+        <v>0.3395398806115439</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Q3 2020$</t>
+          <t>Q3 2020</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.3872106241700768</v>
+        <v>0.5449564712044563</v>
       </c>
       <c r="C9" t="n">
-        <v>0.3741865488968548</v>
+        <v>1.428444879444643</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2000375877467541</v>
+        <v>0.713969258209547</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0565837136295135</v>
+        <v>0.3257092640157674</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Q4 2020$</t>
+          <t>Q4 2020</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9517252630015256</v>
+        <v>0.6656359317161844</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7764860007483073</v>
+        <v>0.9945465253977196</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1569077231924765</v>
+        <v>0.5490062612939669</v>
       </c>
       <c r="E10" t="n">
-        <v>0.06457057527916107</v>
+        <v>0.3343200114418086</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Q1 2021$</t>
+          <t>Q1 2021</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.8364124107374176</v>
+        <v>0.6394326790202198</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8410904667681917</v>
+        <v>0.7903392530878948</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2182757254376686</v>
+        <v>0.5641744746785298</v>
       </c>
       <c r="E11" t="n">
-        <v>0.08889680804144297</v>
+        <v>0.3338690306575793</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Q2 2021$</t>
+          <t>Q2 2021</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.6870846702938616</v>
+        <v>0.5499030255340499</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6442066544213365</v>
+        <v>0.6631425388183607</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2441243473183346</v>
+        <v>0.5244735419505069</v>
       </c>
       <c r="E12" t="n">
-        <v>0.09850785258039246</v>
+        <v>0.33462970462644</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Q3 2021$</t>
+          <t>Q3 2021</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.8704309904264185</v>
+        <v>0.4739436644373797</v>
       </c>
       <c r="C13" t="n">
-        <v>0.799445408756067</v>
+        <v>0.5850249005666273</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2433034629081823</v>
+        <v>0.4510081718839272</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1094702111406576</v>
+        <v>0.3379743942214892</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Q4 2021$</t>
+          <t>Q4 2021</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.868098094806637</v>
+        <v>0.481250667138948</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8262449763178799</v>
+        <v>0.5492101456520386</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2671368870465823</v>
+        <v>0.419497192063879</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1271978552072722</v>
+        <v>0.3408811792555912</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Q1 2022$</t>
+          <t>Q1 2022</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.8819763659110874</v>
+        <v>0.4861263726029907</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8034978834033979</v>
+        <v>0.5220886387941499</v>
       </c>
       <c r="D15" t="n">
-        <v>0.285579507322402</v>
+        <v>0.4228322453919932</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1406450927711149</v>
+        <v>0.3435454231495588</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Q2 2022$</t>
+          <t>Q2 2022</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.9270804313309982</v>
+        <v>0.4617416225808446</v>
       </c>
       <c r="C16" t="n">
-        <v>0.8832650146449619</v>
+        <v>0.4955214444981157</v>
       </c>
       <c r="D16" t="n">
-        <v>0.3043662567912191</v>
+        <v>0.4140146534186994</v>
       </c>
       <c r="E16" t="n">
-        <v>0.1551435413676356</v>
+        <v>0.3459421919281677</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Q3 2022$</t>
+          <t>Q3 2022</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.9431575026613725</v>
+        <v>0.4429031399077412</v>
       </c>
       <c r="C17" t="n">
-        <v>0.8942913314949245</v>
+        <v>0.4754453870865816</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3260961671348564</v>
+        <v>0.3950978251922602</v>
       </c>
       <c r="E17" t="n">
-        <v>0.1712667131533387</v>
+        <v>0.3479488585916479</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Q4 2022$</t>
+          <t>Q4 2022</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.9640884768147756</v>
+        <v>0.4300569271249406</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9132624734110835</v>
+        <v>0.4591209121674681</v>
       </c>
       <c r="D18" t="n">
-        <v>0.341233834242858</v>
+        <v>0.3867267274047179</v>
       </c>
       <c r="E18" t="n">
-        <v>0.186123156656745</v>
+        <v>0.3497068064234699</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Q1 2023$</t>
+          <t>Q1 2023</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.987997253705986</v>
+        <v>0.4199716787195968</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9521503760350231</v>
+        <v>0.4444740153276895</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3597660868729666</v>
+        <v>0.3858679692419142</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2017030223323491</v>
+        <v>0.3512181014165098</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Q2 2023$</t>
+          <t>Q2 2023</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.007005307736014</v>
+        <v>0.4094504198574394</v>
       </c>
       <c r="C20" t="n">
-        <v>0.9653850256644534</v>
+        <v>0.4313726624522503</v>
       </c>
       <c r="D20" t="n">
-        <v>0.3792625954422021</v>
+        <v>0.3818286423547494</v>
       </c>
       <c r="E20" t="n">
-        <v>0.2174969867751969</v>
+        <v>0.3524718136786171</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Q3 2023$</t>
+          <t>Q3 2023</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.026042374667944</v>
+        <v>0.3993059629861925</v>
       </c>
       <c r="C21" t="n">
-        <v>0.9886710686729988</v>
+        <v>0.4194237022554943</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3957219450828781</v>
+        <v>0.3758359617018224</v>
       </c>
       <c r="E21" t="n">
-        <v>0.2330130874462193</v>
+        <v>0.3534973479135821</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Q4 2023$</t>
+          <t>Q4 2023</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1.044818160361264</v>
+        <v>0.3920267936153891</v>
       </c>
       <c r="C22" t="n">
-        <v>1.011563908283502</v>
+        <v>0.4092583715129271</v>
       </c>
       <c r="D22" t="n">
-        <v>0.4129124056937087</v>
+        <v>0.3725651627338414</v>
       </c>
       <c r="E22" t="n">
-        <v>0.2488549489301529</v>
+        <v>0.3543371273321602</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Q1 2024$</t>
+          <t>Q1 2024</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1.062839267576031</v>
+        <v>0.3866437324893752</v>
       </c>
       <c r="C23" t="n">
-        <v>1.027756370159693</v>
+        <v>0.4008747531416141</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4302062081106044</v>
+        <v>0.3710718402870521</v>
       </c>
       <c r="E23" t="n">
-        <v>0.2646687096849225</v>
+        <v>0.3550377706472655</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Q2 2024$</t>
+          <t>Q2 2024</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1.080698151074239</v>
+        <v>0.3815354709359833</v>
       </c>
       <c r="C24" t="n">
-        <v>1.048351658533007</v>
+        <v>0.3935086634951455</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4469976208675631</v>
+        <v>0.3689620342107532</v>
       </c>
       <c r="E24" t="n">
-        <v>0.2804771253750217</v>
+        <v>0.3556134897586724</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Q3 2024$</t>
+          <t>Q3 2024</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1.098133659376456</v>
+        <v>0.377077635881538</v>
       </c>
       <c r="C25" t="n">
-        <v>1.066505221777405</v>
+        <v>0.3872582702529465</v>
       </c>
       <c r="D25" t="n">
-        <v>0.4637871509092154</v>
+        <v>0.3666308393821051</v>
       </c>
       <c r="E25" t="n">
-        <v>0.2963990633157498</v>
+        <v>0.3560772666050629</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Q4 2024$</t>
+          <t>Q4 2024</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1.11525295065664</v>
+        <v>0.3737445216481247</v>
       </c>
       <c r="C26" t="n">
-        <v>1.083611540036914</v>
+        <v>0.382184298024455</v>
       </c>
       <c r="D26" t="n">
-        <v>0.4802609663331708</v>
+        <v>0.3651331201992724</v>
       </c>
       <c r="E26" t="n">
-        <v>0.3122962481376242</v>
+        <v>0.3564589122904928</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Q1 2025$</t>
+          <t>Q1 2025</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1.132288895303013</v>
+        <v>0.3711149410618871</v>
       </c>
       <c r="C27" t="n">
-        <v>1.101860265241368</v>
+        <v>0.3779704759810946</v>
       </c>
       <c r="D27" t="n">
-        <v>0.4967504087991131</v>
+        <v>0.3641487431660444</v>
       </c>
       <c r="E27" t="n">
-        <v>0.3282270177231711</v>
+        <v>0.3567751538060301</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Q2 2025$</t>
+          <t>Q2 2025</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1.149139760672082</v>
+        <v>0.368801882201169</v>
       </c>
       <c r="C28" t="n">
-        <v>1.118800568416478</v>
+        <v>0.3744596304291303</v>
       </c>
       <c r="D28" t="n">
-        <v>0.5132447779092303</v>
+        <v>0.36311204835549</v>
       </c>
       <c r="E28" t="n">
-        <v>0.3441920121673513</v>
+        <v>0.357033502116559</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Q3 2025$</t>
+          <t>Q3 2025</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1.165806158907626</v>
+        <v>0.3668570920831674</v>
       </c>
       <c r="C29" t="n">
-        <v>1.135788815436465</v>
+        <v>0.3715618091135703</v>
       </c>
       <c r="D29" t="n">
-        <v>0.5295359919589511</v>
+        <v>0.3621421965634748</v>
       </c>
       <c r="E29" t="n">
-        <v>0.3601540249885035</v>
+        <v>0.3572447183045518</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Q4 2025$</t>
+          <t>Q4 2025</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1.182379147197616</v>
+        <v>0.3653358537959684</v>
       </c>
       <c r="C30" t="n">
-        <v>1.152835363075652</v>
+        <v>0.369188936447792</v>
       </c>
       <c r="D30" t="n">
-        <v>0.5458124115856439</v>
+        <v>0.3614510230013094</v>
       </c>
       <c r="E30" t="n">
-        <v>0.376138730392536</v>
+        <v>0.3574185979830088</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Q1 2026$</t>
+          <t>Q1 2026</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1.198869633438416</v>
+        <v>0.3641064195189391</v>
       </c>
       <c r="C31" t="n">
-        <v>1.169400899850468</v>
+        <v>0.3672504804985987</v>
       </c>
       <c r="D31" t="n">
-        <v>0.5620783516214136</v>
+        <v>0.360931770810437</v>
       </c>
       <c r="E31" t="n">
-        <v>0.392133775400019</v>
+        <v>0.3575620753469036</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Q2 2026$</t>
+          <t>Q2 2026</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1.215276941483852</v>
+        <v>0.3630584604805778</v>
       </c>
       <c r="C32" t="n">
-        <v>1.186051037870057</v>
+        <v>0.3656458770444848</v>
       </c>
       <c r="D32" t="n">
-        <v>0.5782827517487286</v>
+        <v>0.3604507824454752</v>
       </c>
       <c r="E32" t="n">
-        <v>0.4081335908708137</v>
+        <v>0.3576800412029104</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Q3 2026$</t>
+          <t>Q3 2026</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1.23161603390455</v>
+        <v>0.3621881907178166</v>
       </c>
       <c r="C33" t="n">
-        <v>1.202572787084622</v>
+        <v>0.3643236168463379</v>
       </c>
       <c r="D33" t="n">
-        <v>0.5944629261942574</v>
+        <v>0.3600321380901917</v>
       </c>
       <c r="E33" t="n">
-        <v>0.4241446258157807</v>
+        <v>0.3577767497126343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working final draft, scroll instructions updated
</commit_message>
<xml_diff>
--- a/server/econ_model/data/output_data/simulation_full_irfs_weblab.xlsx
+++ b/server/econ_model/data/output_data/simulation_full_irfs_weblab.xlsx
@@ -546,13 +546,13 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>7.67906559498353</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5611116717935283</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2247201262549182</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -562,16 +562,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1738722793249711</v>
+        <v>2.126180620310202</v>
       </c>
       <c r="C7" t="n">
-        <v>4.202493577422769</v>
+        <v>0.784399373242246</v>
       </c>
       <c r="D7" t="n">
-        <v>1.489088372285891</v>
+        <v>0.0573163021242165</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3912824475614967</v>
+        <v>0.02295465822097256</v>
       </c>
     </row>
     <row r="8">
@@ -581,16 +581,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5150643219552331</v>
+        <v>1.250823269219797</v>
       </c>
       <c r="C8" t="n">
-        <v>2.38438084022046</v>
+        <v>0.8682420686956385</v>
       </c>
       <c r="D8" t="n">
-        <v>1.085193212321585</v>
+        <v>0.1841824810008074</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3395398806115439</v>
+        <v>0.05281454692149209</v>
       </c>
     </row>
     <row r="9">
@@ -600,16 +600,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.5449564712044563</v>
+        <v>-0.7249110131230767</v>
       </c>
       <c r="C9" t="n">
-        <v>1.428444879444643</v>
+        <v>0.2089224047030664</v>
       </c>
       <c r="D9" t="n">
-        <v>0.713969258209547</v>
+        <v>0.1758877094342518</v>
       </c>
       <c r="E9" t="n">
-        <v>0.3257092640157674</v>
+        <v>0.04900679311526703</v>
       </c>
     </row>
     <row r="10">
@@ -619,16 +619,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.6656359317161844</v>
+        <v>0.6865159753608333</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9945465253977196</v>
+        <v>0.5903296160842122</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5490062612939669</v>
+        <v>0.1151690739365489</v>
       </c>
       <c r="E10" t="n">
-        <v>0.3343200114418086</v>
+        <v>0.05209297545338792</v>
       </c>
     </row>
     <row r="11">
@@ -638,16 +638,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.6394326790202198</v>
+        <v>0.5025515255606418</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7903392530878948</v>
+        <v>0.5959011204956751</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5641744746785298</v>
+        <v>0.1650201687880861</v>
       </c>
       <c r="E11" t="n">
-        <v>0.3338690306575793</v>
+        <v>0.071209910670331</v>
       </c>
     </row>
     <row r="12">
@@ -657,16 +657,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.5499030255340499</v>
+        <v>0.3029686325610219</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6631425388183607</v>
+        <v>0.3394271960992525</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5244735419505069</v>
+        <v>0.1743667737899435</v>
       </c>
       <c r="E12" t="n">
-        <v>0.33462970462644</v>
+        <v>0.07369996414224737</v>
       </c>
     </row>
     <row r="13">
@@ -676,16 +676,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4739436644373797</v>
+        <v>0.4560180894374765</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5850249005666273</v>
+        <v>0.4607232308240579</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4510081718839272</v>
+        <v>0.1561092120007968</v>
       </c>
       <c r="E13" t="n">
-        <v>0.3379743942214892</v>
+        <v>0.0772923262882878</v>
       </c>
     </row>
     <row r="14">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.481250667138948</v>
+        <v>0.4080833848739472</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5492101456520386</v>
+        <v>0.4414504753034648</v>
       </c>
       <c r="D14" t="n">
-        <v>0.419497192063879</v>
+        <v>0.1643317149391173</v>
       </c>
       <c r="E14" t="n">
-        <v>0.3408811792555912</v>
+        <v>0.08729073772607357</v>
       </c>
     </row>
     <row r="15">
@@ -714,16 +714,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.4861263726029907</v>
+        <v>0.3811533174910029</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5220886387941499</v>
+        <v>0.3745583348586364</v>
       </c>
       <c r="D15" t="n">
-        <v>0.4228322453919932</v>
+        <v>0.1663411637210251</v>
       </c>
       <c r="E15" t="n">
-        <v>0.3435454231495588</v>
+        <v>0.09200890151730887</v>
       </c>
     </row>
     <row r="16">
@@ -733,16 +733,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.4617416225808446</v>
+        <v>0.3881420511618133</v>
       </c>
       <c r="C16" t="n">
-        <v>0.4955214444981157</v>
+        <v>0.4168696326143367</v>
       </c>
       <c r="D16" t="n">
-        <v>0.4140146534186994</v>
+        <v>0.1684937968177397</v>
       </c>
       <c r="E16" t="n">
-        <v>0.3459421919281677</v>
+        <v>0.09730645996209873</v>
       </c>
     </row>
     <row r="17">
@@ -752,16 +752,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.4429031399077412</v>
+        <v>0.3654049173760063</v>
       </c>
       <c r="C17" t="n">
-        <v>0.4754453870865816</v>
+        <v>0.3862089862028655</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3950978251922602</v>
+        <v>0.173374327479603</v>
       </c>
       <c r="E17" t="n">
-        <v>0.3479488585916479</v>
+        <v>0.103698985751592</v>
       </c>
     </row>
     <row r="18">
@@ -771,16 +771,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.4300569271249406</v>
+        <v>0.3497953997918087</v>
       </c>
       <c r="C18" t="n">
-        <v>0.4591209121674681</v>
+        <v>0.366559229498738</v>
       </c>
       <c r="D18" t="n">
-        <v>0.3867267274047179</v>
+        <v>0.1711745618396443</v>
       </c>
       <c r="E18" t="n">
-        <v>0.3497068064234699</v>
+        <v>0.108185530679839</v>
       </c>
     </row>
     <row r="19">
@@ -790,16 +790,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.4199716787195968</v>
+        <v>0.3387246367038387</v>
       </c>
       <c r="C19" t="n">
-        <v>0.4444740153276895</v>
+        <v>0.368791209172804</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3858679692419142</v>
+        <v>0.1725893582857884</v>
       </c>
       <c r="E19" t="n">
-        <v>0.3512181014165098</v>
+        <v>0.1129468432874593</v>
       </c>
     </row>
     <row r="20">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.4094504198574394</v>
+        <v>0.3238602270634821</v>
       </c>
       <c r="C20" t="n">
-        <v>0.4313726624522503</v>
+        <v>0.3451467378849538</v>
       </c>
       <c r="D20" t="n">
-        <v>0.3818286423547494</v>
+        <v>0.1748269310264452</v>
       </c>
       <c r="E20" t="n">
-        <v>0.3524718136786171</v>
+        <v>0.1174461234015612</v>
       </c>
     </row>
     <row r="21">
@@ -828,16 +828,16 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.3993059629861925</v>
+        <v>0.3105112712890644</v>
       </c>
       <c r="C21" t="n">
-        <v>0.4194237022554943</v>
+        <v>0.3339181071050038</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3758359617018224</v>
+        <v>0.1738035875644765</v>
       </c>
       <c r="E21" t="n">
-        <v>0.3534973479135821</v>
+        <v>0.1212176117324274</v>
       </c>
     </row>
     <row r="22">
@@ -847,16 +847,16 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.3920267936153891</v>
+        <v>0.2982359298534776</v>
       </c>
       <c r="C22" t="n">
-        <v>0.4092583715129271</v>
+        <v>0.3234191360050065</v>
       </c>
       <c r="D22" t="n">
-        <v>0.3725651627338414</v>
+        <v>0.1736136894188594</v>
       </c>
       <c r="E22" t="n">
-        <v>0.3543371273321602</v>
+        <v>0.1249377120431182</v>
       </c>
     </row>
     <row r="23">
@@ -866,16 +866,16 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.3866437324893752</v>
+        <v>0.2864334440828969</v>
       </c>
       <c r="C23" t="n">
-        <v>0.4008747531416141</v>
+        <v>0.3072696842806969</v>
       </c>
       <c r="D23" t="n">
-        <v>0.3710718402870521</v>
+        <v>0.1735461228938694</v>
       </c>
       <c r="E23" t="n">
-        <v>0.3550377706472655</v>
+        <v>0.1282577015935761</v>
       </c>
     </row>
     <row r="24">
@@ -885,16 +885,16 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.3815354709359833</v>
+        <v>0.2756489831728153</v>
       </c>
       <c r="C24" t="n">
-        <v>0.3935086634951455</v>
+        <v>0.2971380042259417</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3689620342107532</v>
+        <v>0.1729829233614411</v>
       </c>
       <c r="E24" t="n">
-        <v>0.3556134897586724</v>
+        <v>0.1312403471243177</v>
       </c>
     </row>
     <row r="25">
@@ -904,16 +904,16 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.377077635881538</v>
+        <v>0.2655195931577507</v>
       </c>
       <c r="C25" t="n">
-        <v>0.3872582702529465</v>
+        <v>0.2855777670477455</v>
       </c>
       <c r="D25" t="n">
-        <v>0.3666308393821051</v>
+        <v>0.1724741610669492</v>
       </c>
       <c r="E25" t="n">
-        <v>0.3560772666050629</v>
+        <v>0.134038250352614</v>
       </c>
     </row>
     <row r="26">
@@ -923,16 +923,16 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.3737445216481247</v>
+        <v>0.2560869251221592</v>
       </c>
       <c r="C26" t="n">
-        <v>0.382184298024455</v>
+        <v>0.2741263086024796</v>
       </c>
       <c r="D26" t="n">
-        <v>0.3651331201992724</v>
+        <v>0.1717005603842099</v>
       </c>
       <c r="E26" t="n">
-        <v>0.3564589122904928</v>
+        <v>0.136531610139227</v>
       </c>
     </row>
     <row r="27">
@@ -942,16 +942,16 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.3711149410618871</v>
+        <v>0.2475141772563171</v>
       </c>
       <c r="C27" t="n">
-        <v>0.3779704759810946</v>
+        <v>0.2649624029466857</v>
       </c>
       <c r="D27" t="n">
-        <v>0.3641487431660444</v>
+        <v>0.1710199468117311</v>
       </c>
       <c r="E27" t="n">
-        <v>0.3567751538060301</v>
+        <v>0.1388092187108512</v>
       </c>
     </row>
     <row r="28">
@@ -961,16 +961,16 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.368801882201169</v>
+        <v>0.2396136248997542</v>
       </c>
       <c r="C28" t="n">
-        <v>0.3744596304291303</v>
+        <v>0.2554064658271269</v>
       </c>
       <c r="D28" t="n">
-        <v>0.36311204835549</v>
+        <v>0.1704123212406752</v>
       </c>
       <c r="E28" t="n">
-        <v>0.357033502116559</v>
+        <v>0.1408932912839464</v>
       </c>
     </row>
     <row r="29">
@@ -980,16 +980,16 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.3668570920831674</v>
+        <v>0.2323186606453229</v>
       </c>
       <c r="C29" t="n">
-        <v>0.3715618091135703</v>
+        <v>0.2468540662644013</v>
       </c>
       <c r="D29" t="n">
-        <v>0.3621421965634748</v>
+        <v>0.1696623031663285</v>
       </c>
       <c r="E29" t="n">
-        <v>0.3572447183045518</v>
+        <v>0.142765974976704</v>
       </c>
     </row>
     <row r="30">
@@ -999,16 +999,16 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.3653358537959684</v>
+        <v>0.2256597828707805</v>
       </c>
       <c r="C30" t="n">
-        <v>0.369188936447792</v>
+        <v>0.2392152072771483</v>
       </c>
       <c r="D30" t="n">
-        <v>0.3614510230013094</v>
+        <v>0.1689724924763883</v>
       </c>
       <c r="E30" t="n">
-        <v>0.3574185979830088</v>
+        <v>0.144474082883066</v>
       </c>
     </row>
     <row r="31">
@@ -1018,16 +1018,16 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.3641064195189391</v>
+        <v>0.2195842908245022</v>
       </c>
       <c r="C31" t="n">
-        <v>0.3672504804985987</v>
+        <v>0.23185922332425</v>
       </c>
       <c r="D31" t="n">
-        <v>0.360931770810437</v>
+        <v>0.1683411832645194</v>
       </c>
       <c r="E31" t="n">
-        <v>0.3575620753469036</v>
+        <v>0.1460217196022424</v>
       </c>
     </row>
     <row r="32">
@@ -1037,16 +1037,16 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.3630584604805778</v>
+        <v>0.2140331697874881</v>
       </c>
       <c r="C32" t="n">
-        <v>0.3656458770444848</v>
+        <v>0.2253234390114134</v>
       </c>
       <c r="D32" t="n">
-        <v>0.3604507824454752</v>
+        <v>0.1677114650653823</v>
       </c>
       <c r="E32" t="n">
-        <v>0.3576800412029104</v>
+        <v>0.1474193631128129</v>
       </c>
     </row>
     <row r="33">
@@ -1056,16 +1056,16 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.3621881907178166</v>
+        <v>0.208968945229438</v>
       </c>
       <c r="C33" t="n">
-        <v>0.3643236168463379</v>
+        <v>0.2193128443248374</v>
       </c>
       <c r="D33" t="n">
-        <v>0.3600321380901917</v>
+        <v>0.1671204930043731</v>
       </c>
       <c r="E33" t="n">
-        <v>0.3577767497126343</v>
+        <v>0.1486884617464986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>